<commit_message>
ok NOW it works
</commit_message>
<xml_diff>
--- a/horario_guardado.xlsx
+++ b/horario_guardado.xlsx
@@ -414,14 +414,153 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:AU1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="n">
+        <v>257</v>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>DEI</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>Redes de Computadoras II</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>---</t>
+        </is>
+      </c>
+      <c r="E1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>IIN</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>-- --</t>
+        </is>
+      </c>
+      <c r="H1" t="n">
+        <v>2008</v>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>TQ</t>
+        </is>
+      </c>
+      <c r="K1" t="inlineStr">
+        <is>
+          <t>EDUCA</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>Ms.</t>
+        </is>
+      </c>
+      <c r="M1" t="inlineStr">
+        <is>
+          <t>Amarilla Fleitas</t>
+        </is>
+      </c>
+      <c r="N1" t="inlineStr">
+        <is>
+          <t>Gustavo Osman</t>
+        </is>
+      </c>
+      <c r="O1" t="inlineStr">
+        <is>
+          <t>gamarilla@pol.una.py</t>
+        </is>
+      </c>
+      <c r="P1" t="inlineStr">
+        <is>
+          <t>Mie 03/09/25</t>
+        </is>
+      </c>
+      <c r="Q1" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="S1" t="inlineStr">
+        <is>
+          <t>Mie 29/10/25</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="V1" t="inlineStr">
+        <is>
+          <t>Mie 19/11/25</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AA1" t="inlineStr">
+        <is>
+          <t>Mie 03/12/25</t>
+        </is>
+      </c>
+      <c r="AB1" s="1" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="AF1" t="inlineStr">
+        <is>
+          <t>Ms. Gustavo Osman Amarilla Fleitas</t>
+        </is>
+      </c>
+      <c r="AG1" t="inlineStr">
+        <is>
+          <t>Ms. Claudio Nil Barúa Acosta</t>
+        </is>
+      </c>
+      <c r="AH1" t="inlineStr">
+        <is>
+          <t>Lic. María Luisa Guanes Romero</t>
+        </is>
+      </c>
+      <c r="AO1" t="inlineStr">
+        <is>
+          <t>I02</t>
+        </is>
+      </c>
+      <c r="AP1" t="inlineStr">
+        <is>
+          <t>14:15 - 16:30</t>
+        </is>
+      </c>
+      <c r="AS1" t="inlineStr">
+        <is>
+          <t>I02</t>
+        </is>
+      </c>
+      <c r="AT1" t="inlineStr">
+        <is>
+          <t>07:30 - 10:30</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>